<commit_message>
All analysis about marketing data
</commit_message>
<xml_diff>
--- a/Marketing Team Data(result) (Recovered).xlsx
+++ b/Marketing Team Data(result) (Recovered).xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
-  <workbookPr/>
+  <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Documents\Execelerate DA Internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6F7643-CC97-4902-A7D9-DEA96F4C2AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8854760-0B5E-4F8C-942D-FBA81BBE9957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost spent per campaign" sheetId="6" r:id="rId1"/>
@@ -23,8 +23,8 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="13" r:id="rId8"/>
-    <pivotCache cacheId="4" r:id="rId9"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
+    <pivotCache cacheId="1" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -242,8 +242,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="\$#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -339,12 +340,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,6 +792,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="12849008"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -849,6 +851,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="12848048"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -972,16 +975,48 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-IN" b="1"/>
+              <a:rPr lang="en-IN" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:rPr>
               <a:t>Cost</a:t>
             </a:r>
             <a:r>
+              <a:rPr lang="en-IN" b="1" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> spent</a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="en-IN" b="1" baseline="0"/>
-              <a:t> spent and click rate of each campaign</a:t>
+              <a:t> and </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IN" b="1" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>click rate</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IN" b="1" baseline="0"/>
+              <a:t> of each campaign</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.2389614078090985"/>
+          <c:y val="7.857142857142857E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1086,14 +1121,21 @@
         <c:dLbl>
           <c:idx val="0"/>
           <c:spPr>
-            <a:noFill/>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF"/>
+            </a:solidFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:srgbClr val="000000">
+                  <a:lumMod val="25000"/>
+                  <a:lumOff val="75000"/>
+                </a:srgbClr>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
               <a:spAutoFit/>
             </a:bodyPr>
             <a:lstStyle/>
@@ -1101,9 +1143,81 @@
               <a:pPr>
                 <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <a:prstGeom prst="wedgeRectCallout">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+              </c15:spPr>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000">
+                  <a:lumMod val="25000"/>
+                  <a:lumOff val="75000"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -1121,7 +1235,678 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <a:prstGeom prst="wedgeRectCallout">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+              </c15:spPr>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000">
+                  <a:lumMod val="25000"/>
+                  <a:lumOff val="75000"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <a:prstGeom prst="wedgeRectCallout">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+              </c15:spPr>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000">
+                  <a:lumMod val="25000"/>
+                  <a:lumOff val="75000"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <a:prstGeom prst="wedgeRectCallout">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+              </c15:spPr>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout>
+            <c:manualLayout>
+              <c:x val="0.14570007107320526"/>
+              <c:y val="-0.15"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000">
+                  <a:lumMod val="25000"/>
+                  <a:lumOff val="75000"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <a:prstGeom prst="wedgeRectCallout">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+              </c15:spPr>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout>
+            <c:manualLayout>
+              <c:x val="6.3965884861407252E-2"/>
+              <c:y val="-0.14285714285714285"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <a:prstGeom prst="wedgeRectCallout">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+              </c15:spPr>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout>
+            <c:manualLayout>
+              <c:x val="7.4626865671641729E-2"/>
+              <c:y val="-0.16190476190476191"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <a:prstGeom prst="wedgeRectCallout">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+              </c15:spPr>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout>
+            <c:manualLayout>
+              <c:x val="7.9957356076759065E-2"/>
+              <c:y val="-0.28571428571428575"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <a:prstGeom prst="wedgeRectCallout">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+              </c15:spPr>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout>
+            <c:manualLayout>
+              <c:x val="0.13148542999289262"/>
+              <c:y val="-0.22857142857142862"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000">
+                  <a:lumMod val="25000"/>
+                  <a:lumOff val="75000"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <a:prstGeom prst="wedgeRectCallout">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+              </c15:spPr>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout>
+            <c:manualLayout>
+              <c:x val="3.9090262970859983E-2"/>
+              <c:y val="-0.26666666666666666"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <a:prstGeom prst="wedgeRectCallout">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+              </c15:spPr>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout>
+            <c:manualLayout>
+              <c:x val="7.4626865671641784E-2"/>
+              <c:y val="-0.3166666666666666"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <a:prstGeom prst="wedgeRectCallout">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+              </c15:spPr>
+            </c:ext>
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
@@ -1132,9 +1917,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.3885045159796182E-2"/>
-          <c:y val="0.19889872013421003"/>
-          <c:w val="0.65405051046008955"/>
+          <c:x val="0.11942159282328516"/>
+          <c:y val="0.2060416197975253"/>
+          <c:w val="0.79264322370151497"/>
           <c:h val="0.54451172984820195"/>
         </c:manualLayout>
       </c:layout>
@@ -1279,6 +2064,551 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-6B7C-4BB3-92E7-343415627523}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-6B7C-4BB3-92E7-343415627523}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-6B7C-4BB3-92E7-343415627523}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-6B7C-4BB3-92E7-343415627523}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="7.4626865671641784E-2"/>
+                  <c:y val="-0.3166666666666666"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:prstGeom prst="wedgeRectCallout">
+                      <a:avLst/>
+                    </a:prstGeom>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                  </c15:spPr>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-6B7C-4BB3-92E7-343415627523}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.9090262970859983E-2"/>
+                  <c:y val="-0.26666666666666666"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:prstGeom prst="wedgeRectCallout">
+                      <a:avLst/>
+                    </a:prstGeom>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                  </c15:spPr>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-6B7C-4BB3-92E7-343415627523}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.13148542999289262"/>
+                  <c:y val="-0.22857142857142862"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-6B7C-4BB3-92E7-343415627523}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="7.9957356076759065E-2"/>
+                  <c:y val="-0.28571428571428575"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:prstGeom prst="wedgeRectCallout">
+                      <a:avLst/>
+                    </a:prstGeom>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                  </c15:spPr>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-6B7C-4BB3-92E7-343415627523}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="7.4626865671641729E-2"/>
+                  <c:y val="-0.16190476190476191"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:prstGeom prst="wedgeRectCallout">
+                      <a:avLst/>
+                    </a:prstGeom>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                  </c15:spPr>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-6B7C-4BB3-92E7-343415627523}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="6.3965884861407252E-2"/>
+                  <c:y val="-0.14285714285714285"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:prstGeom prst="wedgeRectCallout">
+                      <a:avLst/>
+                    </a:prstGeom>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                  </c15:spPr>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-6B7C-4BB3-92E7-343415627523}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.14570007107320526"/>
+                  <c:y val="-0.15"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-6B7C-4BB3-92E7-343415627523}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-6B7C-4BB3-92E7-343415627523}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-6B7C-4BB3-92E7-343415627523}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-6B7C-4BB3-92E7-343415627523}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-6B7C-4BB3-92E7-343415627523}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:srgbClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'CTR vs CPR'!$A$36:$A$47</c:f>
@@ -1496,47 +2826,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.75938163405125825"/>
-          <c:y val="0.4014971453310604"/>
-          <c:w val="0.23449091496834951"/>
-          <c:h val="0.22140406418269881"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1583,8 +2872,6 @@
       <c14:pivotOptions>
         <c14:dropZoneFilter val="1"/>
         <c14:dropZoneCategories val="1"/>
-        <c14:dropZoneData val="1"/>
-        <c14:dropZoneSeries val="1"/>
         <c14:dropZonesVisible val="1"/>
       </c14:pivotOptions>
     </c:ext>
@@ -1679,7 +2966,9 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="bg2">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1687,6 +2976,63 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-E7C9-42DA-AE1F-C2B43C795885}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-E7C9-42DA-AE1F-C2B43C795885}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-E7C9-42DA-AE1F-C2B43C795885}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:cat>
             <c:strRef>
               <c:f>'CTR vs CPR'!$A$19:$A$29</c:f>
@@ -1851,9 +3197,8 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -2034,7 +3379,9 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="bg2">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -2042,6 +3389,44 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-E9C9-41BF-8964-4D5DBCB27527}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-E9C9-41BF-8964-4D5DBCB27527}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:cat>
             <c:strRef>
               <c:f>'CTR vs CPR'!$A$2:$A$12</c:f>
@@ -2341,22 +3726,60 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-IN" b="1"/>
+              <a:rPr lang="en-IN" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:rPr>
               <a:t>CPR</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-IN" b="1" baseline="0"/>
-              <a:t> and CPC with UCTR</a:t>
+              <a:t> and </a:t>
             </a:r>
-            <a:endParaRPr lang="en-IN" b="1"/>
+            <a:r>
+              <a:rPr lang="en-IN" b="1" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="FFC000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>CPC</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IN" b="1" baseline="0"/>
+              <a:t> with </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IN" b="1" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>UCTR</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IN" b="1">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.39483953372272623"/>
+          <c:y val="6.6697911439670216E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -2377,7 +3800,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-IN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2458,7 +3881,9 @@
           <c:spPr>
             <a:noFill/>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -2551,6 +3976,380 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="bg2">
+              <a:lumMod val="65000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln cmpd="tri">
+            <a:solidFill>
+              <a:schemeClr val="bg2">
+                <a:lumMod val="65000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="bg2">
+              <a:lumMod val="65000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="bg2">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="bg2">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="bg2">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="bg2">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="bg2">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="bg2">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="bg2">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="12"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="13"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout>
+            <c:manualLayout>
+              <c:x val="8.599749495185828E-2"/>
+              <c:y val="-0.36231915917604024"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:noAutofit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Second</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> least user intreact campaign</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="EA4335"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <a:prstGeom prst="wedgeRectCallout">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+              </c15:spPr>
+              <c15:layout>
+                <c:manualLayout>
+                  <c:w val="0.15363189567169566"/>
+                  <c:h val="0.14505291526622244"/>
+                </c:manualLayout>
+              </c15:layout>
+              <c15:showDataLabelsRange val="0"/>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="14"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="15"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout>
+            <c:manualLayout>
+              <c:x val="0.10290625339069648"/>
+              <c:y val="-0.20274218819719622"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+                  <a:t>It is inefficient due to its high CPR and CTS, combined with a very low CTR."</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" baseline="0"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="EA4335"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <a:prstGeom prst="wedgeRectCallout">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+              </c15:spPr>
+              <c15:showDataLabelsRange val="0"/>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout>
@@ -2558,10 +4357,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18703371538017208"/>
-          <c:y val="0.23333173292362844"/>
-          <c:w val="0.5506257663737979"/>
-          <c:h val="0.48154780957258392"/>
+          <c:x val="0.14256291307617666"/>
+          <c:y val="0.19522621911327157"/>
+          <c:w val="0.77734115208159171"/>
+          <c:h val="0.60452266606370031"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -2592,6 +4391,199 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln cmpd="tri">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="65000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-CB5D-49E6-9F3E-38B0BB086450}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-CB5D-49E6-9F3E-38B0BB086450}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-CB5D-49E6-9F3E-38B0BB086450}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-CB5D-49E6-9F3E-38B0BB086450}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-CB5D-49E6-9F3E-38B0BB086450}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-CB5D-49E6-9F3E-38B0BB086450}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-CB5D-49E6-9F3E-38B0BB086450}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-CB5D-49E6-9F3E-38B0BB086450}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-CB5D-49E6-9F3E-38B0BB086450}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:cat>
             <c:strRef>
               <c:f>'CPR vs UCTR'!$A$4:$A$15</c:f>
@@ -2835,6 +4827,267 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-CB5D-49E6-9F3E-38B0BB086450}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="8.599749495185828E-2"/>
+                  <c:y val="-0.36231915917604024"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:noAutofit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Second</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> least user intreact campaign</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:solidFill>
+                    <a:srgbClr val="EA4335"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:prstGeom prst="wedgeRectCallout">
+                      <a:avLst/>
+                    </a:prstGeom>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                  </c15:spPr>
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.15363189567169566"/>
+                      <c:h val="0.14505291526622244"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-CB5D-49E6-9F3E-38B0BB086450}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.10290625339069648"/>
+                  <c:y val="-0.20274218819719622"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:spAutoFit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+                      <a:t>It is inefficient due to its high CPR and CTS, combined with a very low CTR."</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:solidFill>
+                    <a:srgbClr val="EA4335"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:prstGeom prst="wedgeRectCallout">
+                      <a:avLst/>
+                    </a:prstGeom>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                  </c15:spPr>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-CB5D-49E6-9F3E-38B0BB086450}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'CPR vs UCTR'!$A$4:$A$15</c:f>
@@ -2971,6 +5224,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.54533895316942527"/>
+              <c:y val="0.91870239765471218"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3038,6 +5299,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="128731536"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3099,8 +5361,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="7.2393822393822388E-2"/>
-              <c:y val="0.32579940464758972"/>
+              <c:x val="4.6667251591482932E-2"/>
+              <c:y val="0.31915211002879007"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -3128,7 +5390,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-IN"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3164,6 +5426,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="128734896"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -3174,47 +5437,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.75213824623273429"/>
-          <c:y val="0.39985302904210146"/>
-          <c:w val="0.23820924411475591"/>
-          <c:h val="0.29887091095320401"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -3260,9 +5482,6 @@
     <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
       <c14:pivotOptions>
         <c14:dropZoneFilter val="1"/>
-        <c14:dropZoneCategories val="1"/>
-        <c14:dropZoneData val="1"/>
-        <c14:dropZoneSeries val="1"/>
         <c14:dropZonesVisible val="1"/>
       </c14:pivotOptions>
     </c:ext>
@@ -3345,7 +5564,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-IN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3658,6 +5877,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="476341984"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3716,6 +5936,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="476344384"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -3871,7 +6092,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-IN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4184,6 +6405,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="503699968"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -4242,6 +6464,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="503697568"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -4346,6 +6569,36 @@
   </c:pivotSource>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IN"/>
+              <a:t>No</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IN" baseline="0"/>
+              <a:t> of people who saw ad</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IN"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4433,6 +6686,118 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout>
+            <c:manualLayout>
+              <c:x val="8.771929824561403E-3"/>
+              <c:y val="-0.13051146384479717"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:fld id="{26801080-2148-4B53-96C0-CC05F1A3E850}" type="CATEGORYNAME">
+                  <a:rPr lang="en-US"/>
+                  <a:pPr>
+                    <a:defRPr/>
+                  </a:pPr>
+                  <a:t>[CATEGORY NAME]</a:t>
+                </a:fld>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>, , first less </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000">
+                  <a:lumMod val="25000"/>
+                  <a:lumOff val="75000"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <a:prstGeom prst="wedgeRectCallout">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+              </c15:spPr>
+              <c15:dlblFieldTable/>
+              <c15:showDataLabelsRange val="0"/>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -4464,6 +6829,151 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="8.771929824561403E-3"/>
+                  <c:y val="-0.13051146384479717"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:spAutoFit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:fld id="{26801080-2148-4B53-96C0-CC05F1A3E850}" type="CATEGORYNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[CATEGORY NAME]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>, , first less </a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:solidFill>
+                    <a:srgbClr val="000000">
+                      <a:lumMod val="25000"/>
+                      <a:lumOff val="75000"/>
+                    </a:srgbClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:prstGeom prst="wedgeRectCallout">
+                      <a:avLst/>
+                    </a:prstGeom>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                  </c15:spPr>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-2F94-4C92-8EA2-B0B8E0B47B3D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet4!$A$4:$A$15</c:f>
@@ -4509,7 +7019,7 @@
             <c:numRef>
               <c:f>Sheet4!$B$4:$B$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>8.1522661660000004</c:v>
@@ -4638,7 +7148,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4757,8 +7267,6 @@
     <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
       <c14:pivotOptions>
         <c14:dropZoneFilter val="1"/>
-        <c14:dropZoneCategories val="1"/>
-        <c14:dropZoneData val="1"/>
         <c14:dropZoneSeries val="1"/>
         <c14:dropZonesVisible val="1"/>
       </c14:pivotOptions>
@@ -4870,10 +7378,13 @@
               <a:gradFill rotWithShape="1">
                 <a:gsLst>
                   <a:gs pos="0">
-                    <a:schemeClr val="accent6">
-                      <a:satMod val="103000"/>
-                      <a:lumMod val="102000"/>
-                      <a:tint val="94000"/>
+                    <a:schemeClr val="bg2">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="72750">
+                    <a:schemeClr val="bg2">
+                      <a:lumMod val="75000"/>
                     </a:schemeClr>
                   </a:gs>
                   <a:gs pos="50000">
@@ -4908,6 +7419,100 @@
               </a:effectLst>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.11372549019607843"/>
+                  <c:y val="-0.11702986279257466"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>Reach doesn't affect CTR growth</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-C1D1-4630-B907-6930D16FC6D6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:srgbClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>'Reach vs CTR'!$B$2:$B$34</c:f>
@@ -10296,16 +12901,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>45720</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>99060</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10338,15 +12943,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>10330</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>3654</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:colOff>441960</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10374,15 +12979,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>579120</xdr:colOff>
+      <xdr:colOff>457200</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>556260</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10410,15 +13015,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>594360</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>454462</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10451,15 +13056,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>691497</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>348953</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>135308</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10568,16 +13173,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>251460</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>140970</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>556260</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>34290</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10609,16 +13214,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12068,7 +14673,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A9E7D44F-D942-43F0-ABCF-45E4C4F4A79B}" name="PivotTable2" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="47">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A9E7D44F-D942-43F0-ABCF-45E4C4F4A79B}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="47">
   <location ref="A3:C15" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField axis="axisRow" showAll="0" sortType="descending">
@@ -12182,7 +14787,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F7E437DE-94E6-49AA-BAAB-906252152594}" name="PivotTable4" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="13">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F7E437DE-94E6-49AA-BAAB-906252152594}" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="15">
   <location ref="A35:C47" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField axis="axisRow" showAll="0" sortType="descending">
@@ -12320,7 +14925,7 @@
       </pivotArea>
     </format>
   </formats>
-  <chartFormats count="4">
+  <chartFormats count="15">
     <chartFormat chart="7" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -12357,6 +14962,138 @@
         </references>
       </pivotArea>
     </chartFormat>
+    <chartFormat chart="7" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="6">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="7">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="9">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="10">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
   </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -12371,7 +15108,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{375A1537-4018-45B3-9B92-33486155AEAB}" name="PivotTable3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{375A1537-4018-45B3-9B92-33486155AEAB}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
   <location ref="A3:D15" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField axis="axisRow" showAll="0" sortType="descending">
@@ -12475,7 +15212,7 @@
     <dataField name="Sum of Unique Click-Through Rate (Unique CTR in %)" fld="12" baseField="0" baseItem="0" numFmtId="2"/>
     <dataField name="Sum of Cost Per Click (CPC)" fld="14" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
-  <chartFormats count="6">
+  <chartFormats count="19">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -12530,6 +15267,162 @@
         </references>
       </pivotArea>
     </chartFormat>
+    <chartFormat chart="2" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="6">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="7">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="9">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="10">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="12">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="13">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="15">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
   </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -12544,7 +15437,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D5DAD2C6-D61D-42A5-92EF-43A8E10B4BFF}" name="PivotTable3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D5DAD2C6-D61D-42A5-92EF-43A8E10B4BFF}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A3:C15" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField axis="axisRow" showAll="0" sortType="descending">
@@ -12645,7 +15538,7 @@
     <dataField name="Sum of Click-Through Rate (CTR in %)" fld="11" baseField="0" baseItem="0" numFmtId="2"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="1">
+    <format dxfId="2">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -12666,7 +15559,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="1">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -12709,7 +15602,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ACDD42F3-2292-47E6-A94C-86978B509CBB}" name="PivotTable8" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ACDD42F3-2292-47E6-A94C-86978B509CBB}" name="PivotTable8" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="A3:B15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField axis="axisRow" showAll="0" sortType="descending">
@@ -12799,14 +15692,26 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Sum of Frequency" fld="7" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Frequency" fld="7" baseField="0" baseItem="0" numFmtId="165"/>
   </dataFields>
-  <chartFormats count="1">
+  <chartFormats count="2">
     <chartFormat chart="1" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="7"/>
           </reference>
         </references>
       </pivotArea>
@@ -13365,7 +16270,7 @@
   <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -13731,8 +16636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C25C8A7-D6C5-459B-A9E6-07991FFB12A9}">
   <dimension ref="A3:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView topLeftCell="B1" zoomScale="107" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -13767,7 +16672,7 @@
       <c r="C4" s="9">
         <v>12.729516419999999</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="16">
         <v>23.7644527</v>
       </c>
     </row>
@@ -13781,7 +16686,7 @@
       <c r="C5" s="9">
         <v>10.189331729999999</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="16">
         <v>22.355507249999999</v>
       </c>
     </row>
@@ -13795,7 +16700,7 @@
       <c r="C6" s="9">
         <v>26.063625440000003</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="16">
         <v>14.438605090000001</v>
       </c>
     </row>
@@ -13809,7 +16714,7 @@
       <c r="C7" s="9">
         <v>7.6500061199999987</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="16">
         <v>10.75425815</v>
       </c>
     </row>
@@ -13823,7 +16728,7 @@
       <c r="C8" s="9">
         <v>17.659132390000003</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="16">
         <v>16.512725230000001</v>
       </c>
     </row>
@@ -13837,7 +16742,7 @@
       <c r="C9" s="9">
         <v>17.414205930000001</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="16">
         <v>7.3421097900000003</v>
       </c>
     </row>
@@ -13851,7 +16756,7 @@
       <c r="C10" s="9">
         <v>11.17901958</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="16">
         <v>3.8510243500000003</v>
       </c>
     </row>
@@ -13865,7 +16770,7 @@
       <c r="C11" s="9">
         <v>12.22923314</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="16">
         <v>2.1667277899999999</v>
       </c>
     </row>
@@ -13879,7 +16784,7 @@
       <c r="C12" s="9">
         <v>18.275484119999998</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="16">
         <v>1.24230873</v>
       </c>
     </row>
@@ -13893,7 +16798,7 @@
       <c r="C13" s="9">
         <v>28.078126659999999</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="16">
         <v>1.0427242699999999</v>
       </c>
     </row>
@@ -13907,7 +16812,7 @@
       <c r="C14" s="9">
         <v>8.2752201900000006</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="16">
         <v>1.3488614299999999</v>
       </c>
     </row>
@@ -13921,7 +16826,7 @@
       <c r="C15" s="9">
         <v>169.74290172000002</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="16">
         <v>104.81930478</v>
       </c>
     </row>
@@ -14271,13 +17176,13 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="17" t="s">
         <v>45</v>
       </c>
       <c r="B28" s="13">
         <v>1.0427242699999999</v>
       </c>
-      <c r="C28" s="19">
+      <c r="C28" s="18">
         <v>29.556386891637523</v>
       </c>
     </row>
@@ -14426,8 +17331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48FEA636-8A1B-48A8-84BA-156C6FC82B89}">
   <dimension ref="A3:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -14448,7 +17353,7 @@
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="19">
         <v>8.1522661660000004</v>
       </c>
     </row>
@@ -14456,7 +17361,7 @@
       <c r="A5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="19">
         <v>7.0732353830000001</v>
       </c>
     </row>
@@ -14464,7 +17369,7 @@
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="19">
         <v>4.2464348300000001</v>
       </c>
     </row>
@@ -14472,7 +17377,7 @@
       <c r="A7" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="19">
         <v>4.0751694689999995</v>
       </c>
     </row>
@@ -14480,7 +17385,7 @@
       <c r="A8" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="19">
         <v>3.8720502730000002</v>
       </c>
     </row>
@@ -14488,7 +17393,7 @@
       <c r="A9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="19">
         <v>3.6216787349999997</v>
       </c>
     </row>
@@ -14496,7 +17401,7 @@
       <c r="A10" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="19">
         <v>3.6039657139999997</v>
       </c>
     </row>
@@ -14504,7 +17409,7 @@
       <c r="A11" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="19">
         <v>3.3621250049999998</v>
       </c>
     </row>
@@ -14512,7 +17417,7 @@
       <c r="A12" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="19">
         <v>3.289436861</v>
       </c>
     </row>
@@ -14520,7 +17425,7 @@
       <c r="A13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="19">
         <v>3.2416989030000001</v>
       </c>
     </row>
@@ -14528,7 +17433,7 @@
       <c r="A14" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14" s="19">
         <v>2.263661017</v>
       </c>
     </row>
@@ -14536,7 +17441,7 @@
       <c r="A15" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="19">
         <v>46.801722355999999</v>
       </c>
     </row>
@@ -16299,7 +19204,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>